<commit_message>
except check availiblity it is on perfect condition
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/MOCK_check_availability.xlsx
+++ b/ExportedFiles/excelFiles/MOCK_check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +497,38 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-09-13 19:49:11</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MOCK_check_availability</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MOCKURL_https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MOCK_No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>19:49:11</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
unit test change all logic
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/MOCK_check_availability.xlsx
+++ b/ExportedFiles/excelFiles/MOCK_check_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,38 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-09-29 00:05:44</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MOCK_check_availability</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MOCKURL_https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>MOCK_No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>00:05:44</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>